<commit_message>
investment: add regions in importer
</commit_message>
<xml_diff>
--- a/optaplanner-examples/data/investment/import/irrinki_1.xlsx
+++ b/optaplanner-examples/data/investment/import/irrinki_1.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
   <si>
     <t>Investment parametrization</t>
   </si>
@@ -25,6 +25,18 @@
     <t>Standard deviation maximum</t>
   </si>
   <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Quantity maximum</t>
+  </si>
+  <si>
+    <t>UK</t>
+  </si>
+  <si>
+    <t>Global</t>
+  </si>
+  <si>
     <t>Asset class</t>
   </si>
   <si>
@@ -34,7 +46,7 @@
     <t>ID</t>
   </si>
   <si>
-    <t>Name</t>
+    <t>Region</t>
   </si>
   <si>
     <t>Expected return</t>
@@ -49,10 +61,13 @@
     <t>Ex-UK Equities</t>
   </si>
   <si>
-    <t>Intermediate Bond</t>
+    <t>Intermediate Bonds</t>
   </si>
   <si>
     <t>Long-Term Bonds</t>
+  </si>
+  <si>
+    <t>UK Bonds</t>
   </si>
   <si>
     <t>Real Estate</t>
@@ -112,16 +127,16 @@
     </border>
     <border diagonalDown="false" diagonalUp="false">
       <left/>
-      <right style="hair"/>
+      <right/>
       <top/>
-      <bottom/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
     <border diagonalDown="false" diagonalUp="false">
       <left/>
-      <right/>
+      <right style="hair"/>
       <top/>
-      <bottom style="hair"/>
+      <bottom/>
       <diagonal/>
     </border>
     <border diagonalDown="false" diagonalUp="false">
@@ -163,15 +178,15 @@
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
     </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="4" numFmtId="164" xfId="0">
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="2" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="0" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
     </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="3" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
@@ -200,7 +215,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="G35" activeCellId="0" pane="topLeft" sqref="G35"/>
+      <selection activeCell="B2" activeCellId="0" pane="topLeft" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <cols>
@@ -237,16 +252,43 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+      <selection activeCell="C9" activeCellId="0" pane="topLeft" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5764705882353"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5764705882353"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0509803921569"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5764705882353"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="1" s="3">
+      <c r="A1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2">
+      <c r="A2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
+      <c r="A3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
@@ -262,65 +304,70 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+      <selection activeCell="B10" activeCellId="0" pane="topLeft" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.3921568627451"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.3803921568627"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="14.4274509803922"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="17.9176470588235"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5764705882353"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.4274509803922"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="14.4274509803922"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="4" width="17.9176470588235"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.5764705882353"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="1" s="6">
-      <c r="A1" s="4" t="s">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="1" s="7">
+      <c r="A1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2" s="3">
+      <c r="A2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="5" t="s">
+      <c r="C2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2" s="7">
-      <c r="A2" s="7" t="s">
+      <c r="I2" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="J2" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="F2" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="G2" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="H2" s="7" t="n">
-        <v>4</v>
-      </c>
-      <c r="I2" s="7" t="n">
-        <v>5</v>
-      </c>
-      <c r="J2" s="7" t="n">
+      <c r="K2" s="3" t="n">
         <v>6</v>
       </c>
     </row>
@@ -329,43 +376,46 @@
         <v>1</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="2" t="n">
         <v>0.1</v>
       </c>
-      <c r="D3" s="3" t="n">
+      <c r="E3" s="4" t="n">
         <v>0.15</v>
       </c>
-      <c r="E3" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="F3" s="11" t="inlineStr">
-        <f aca="false">E4</f>
-        <is>
-          <t/>
-        </is>
+      <c r="F3" s="11" t="n">
+        <v>1</v>
       </c>
       <c r="G3" s="11" t="inlineStr">
-        <f aca="false">E5</f>
+        <f aca="false">F4</f>
         <is>
           <t/>
         </is>
       </c>
       <c r="H3" s="11" t="inlineStr">
-        <f aca="false">E6</f>
+        <f aca="false">F5</f>
         <is>
           <t/>
         </is>
       </c>
       <c r="I3" s="11" t="inlineStr">
-        <f aca="false">E7</f>
+        <f aca="false">F6</f>
         <is>
           <t/>
         </is>
       </c>
       <c r="J3" s="11" t="inlineStr">
-        <f aca="false">E8</f>
+        <f aca="false">F7</f>
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="K3" s="11" t="inlineStr">
+        <f aca="false">F8</f>
         <is>
           <t/>
         </is>
@@ -376,40 +426,43 @@
         <v>2</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2" t="n">
         <v>0.08</v>
       </c>
-      <c r="D4" s="3" t="n">
+      <c r="E4" s="4" t="n">
         <v>0.12</v>
       </c>
-      <c r="E4" s="11" t="n">
+      <c r="F4" s="11" t="n">
         <v>0.76</v>
       </c>
-      <c r="F4" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" s="11" t="inlineStr">
-        <f aca="false">F5</f>
-        <is>
-          <t/>
-        </is>
+      <c r="G4" s="11" t="n">
+        <v>1</v>
       </c>
       <c r="H4" s="11" t="inlineStr">
-        <f aca="false">F6</f>
+        <f aca="false">G5</f>
         <is>
           <t/>
         </is>
       </c>
       <c r="I4" s="11" t="inlineStr">
-        <f aca="false">F7</f>
+        <f aca="false">G6</f>
         <is>
           <t/>
         </is>
       </c>
       <c r="J4" s="11" t="inlineStr">
-        <f aca="false">F8</f>
+        <f aca="false">G7</f>
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="K4" s="11" t="inlineStr">
+        <f aca="false">G8</f>
         <is>
           <t/>
         </is>
@@ -420,37 +473,40 @@
         <v>3</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="2" t="n">
         <v>0.04</v>
       </c>
-      <c r="D5" s="3" t="n">
+      <c r="E5" s="4" t="n">
         <v>0.07</v>
       </c>
-      <c r="E5" s="11" t="n">
+      <c r="F5" s="11" t="n">
         <v>0.35</v>
       </c>
-      <c r="F5" s="11" t="n">
+      <c r="G5" s="11" t="n">
         <v>0.04</v>
       </c>
-      <c r="G5" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="H5" s="11" t="inlineStr">
-        <f aca="false">G6</f>
-        <is>
-          <t/>
-        </is>
+      <c r="H5" s="11" t="n">
+        <v>1</v>
       </c>
       <c r="I5" s="11" t="inlineStr">
-        <f aca="false">G7</f>
+        <f aca="false">H6</f>
         <is>
           <t/>
         </is>
       </c>
       <c r="J5" s="11" t="inlineStr">
-        <f aca="false">G8</f>
+        <f aca="false">H7</f>
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="K5" s="11" t="inlineStr">
+        <f aca="false">H8</f>
         <is>
           <t/>
         </is>
@@ -461,34 +517,37 @@
         <v>4</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2" t="n">
         <v>0.045</v>
       </c>
-      <c r="D6" s="3" t="n">
+      <c r="E6" s="4" t="n">
         <v>0.08</v>
       </c>
-      <c r="E6" s="11" t="n">
+      <c r="F6" s="11" t="n">
         <v>0.5</v>
       </c>
-      <c r="F6" s="11" t="n">
+      <c r="G6" s="11" t="n">
         <v>0.3</v>
       </c>
-      <c r="G6" s="11" t="n">
+      <c r="H6" s="11" t="n">
         <v>0.87</v>
       </c>
-      <c r="H6" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="I6" s="11" t="inlineStr">
-        <f aca="false">H7</f>
-        <is>
-          <t/>
-        </is>
+      <c r="I6" s="11" t="n">
+        <v>1</v>
       </c>
       <c r="J6" s="11" t="inlineStr">
-        <f aca="false">H8</f>
+        <f aca="false">I7</f>
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="K6" s="11" t="inlineStr">
+        <f aca="false">I8</f>
         <is>
           <t/>
         </is>
@@ -499,31 +558,34 @@
         <v>5</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="2" t="n">
         <v>0.05</v>
       </c>
-      <c r="D7" s="3" t="n">
+      <c r="E7" s="4" t="n">
         <v>0.09</v>
       </c>
-      <c r="E7" s="11" t="n">
+      <c r="F7" s="11" t="n">
         <v>0.24</v>
       </c>
-      <c r="F7" s="11" t="n">
+      <c r="G7" s="11" t="n">
         <v>0.36</v>
       </c>
-      <c r="G7" s="11" t="n">
+      <c r="H7" s="11" t="n">
         <v>0.62</v>
       </c>
-      <c r="H7" s="11" t="n">
+      <c r="I7" s="11" t="n">
         <v>0.52</v>
       </c>
-      <c r="I7" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="J7" s="11" t="inlineStr">
-        <f aca="false">I8</f>
+      <c r="J7" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="K7" s="11" t="inlineStr">
+        <f aca="false">J8</f>
         <is>
           <t/>
         </is>
@@ -534,37 +596,40 @@
         <v>6</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="2" t="n">
+        <v>17</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="2" t="n">
         <v>0.07</v>
       </c>
-      <c r="D8" s="3" t="n">
+      <c r="E8" s="4" t="n">
         <v>0.1</v>
       </c>
-      <c r="E8" s="11" t="n">
+      <c r="F8" s="11" t="n">
         <v>0.3</v>
       </c>
-      <c r="F8" s="11" t="n">
+      <c r="G8" s="11" t="n">
         <v>0.25</v>
       </c>
-      <c r="G8" s="11" t="n">
+      <c r="H8" s="11" t="n">
         <v>-0.05</v>
       </c>
-      <c r="H8" s="11" t="n">
+      <c r="I8" s="11" t="n">
         <v>-0.02</v>
       </c>
-      <c r="I8" s="11" t="n">
+      <c r="J8" s="11" t="n">
         <v>0.2</v>
       </c>
-      <c r="J8" s="11" t="n">
+      <c r="K8" s="11" t="n">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="E1:J1"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="F1:K1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
[DROOLS-4900] bump to poi 4
</commit_message>
<xml_diff>
--- a/optaplanner-examples/data/investment/import/irrinki_1.xlsx
+++ b/optaplanner-examples/data/investment/import/irrinki_1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="3" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="239" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Parametrization" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,73 +14,78 @@
     <sheet name="AssetClasses" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="21">
   <si>
-    <t>Investment parametrization</t>
-  </si>
-  <si>
-    <t>Standard deviation maximum</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Quantity maximum</t>
-  </si>
-  <si>
-    <t>UK</t>
-  </si>
-  <si>
-    <t>Global</t>
-  </si>
-  <si>
-    <t>Equities</t>
-  </si>
-  <si>
-    <t>Bonds</t>
-  </si>
-  <si>
-    <t>Real Estate</t>
-  </si>
-  <si>
-    <t>Asset class</t>
-  </si>
-  <si>
-    <t>Correlation</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>Region</t>
-  </si>
-  <si>
-    <t>Sector</t>
-  </si>
-  <si>
-    <t>Expected return</t>
-  </si>
-  <si>
-    <t>Standard deviation</t>
-  </si>
-  <si>
-    <t>UK Equities</t>
-  </si>
-  <si>
-    <t>Ex-UK Equities</t>
-  </si>
-  <si>
-    <t>Intermediate Bonds</t>
-  </si>
-  <si>
-    <t>Long-Term Bonds</t>
-  </si>
-  <si>
-    <t>UK Bonds</t>
+    <t xml:space="preserve">Investment parametrization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Standard deviation maximum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quantity maximum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Global</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Equities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bonds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Real Estate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asset class</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Correlation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Region</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expected return</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Standard deviation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UK Equities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ex-UK Equities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intermediate Bonds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Long-Term Bonds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UK Bonds</t>
   </si>
 </sst>
 </file>
@@ -88,42 +93,37 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt formatCode="GENERAL" numFmtId="164"/>
-    <numFmt formatCode="0.00%" numFmtId="165"/>
+    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="0.00%"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <sz val="10"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <sz val="10"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <sz val="10"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <sz val="10"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <charset val="1"/>
-      <family val="2"/>
       <b val="true"/>
       <sz val="10"/>
-    </font>
-    <font>
       <name val="Arial"/>
       <family val="2"/>
-      <sz val="10"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -135,28 +135,28 @@
     </fill>
   </fills>
   <borders count="4">
-    <border diagonalDown="false" diagonalUp="false">
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom style="hair"/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right style="hair"/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right style="hair"/>
       <top/>
@@ -165,63 +165,91 @@
     </border>
   </borders>
   <cellStyleXfs count="20">
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="2" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="4" numFmtId="165" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="3" fillId="0" fontId="4" numFmtId="165" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0"/>
+  <cellXfs count="13">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
-    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
-    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
-    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
-    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -233,21 +261,22 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B2" activeCellId="0" pane="topLeft" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.3058823529412"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.6313725490196"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.64"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1">
+    <row r="1" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="2">
+    <row r="2" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>1</v>
       </c>
@@ -258,7 +287,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="true" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -273,17 +302,18 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C9" activeCellId="0" pane="topLeft" sqref="C9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6313725490196"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.1411764705882"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.6313725490196"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.64"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1" s="3">
+    <row r="1" s="3" customFormat="true" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -291,7 +321,7 @@
         <v>3</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="2">
+    <row r="2" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>4</v>
       </c>
@@ -299,7 +329,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="3">
+    <row r="3" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>5</v>
       </c>
@@ -310,7 +340,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -325,17 +355,18 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B3" activeCellId="0" pane="topLeft" sqref="B3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6313725490196"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.1411764705882"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.6313725490196"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.64"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1" s="3">
+    <row r="1" s="3" customFormat="true" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -343,7 +374,7 @@
         <v>3</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="2">
+    <row r="2" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
@@ -351,7 +382,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="3">
+    <row r="3" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
@@ -359,7 +390,7 @@
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="4">
+    <row r="4" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>8</v>
       </c>
@@ -370,7 +401,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -385,20 +416,21 @@
   </sheetPr>
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B10" activeCellId="0" pane="topLeft" sqref="B10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L29" activeCellId="0" sqref="L29"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.4078431372549"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.4588235294118"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="14.4980392156863"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="14.4980392156863"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="18.0078431372549"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.6313725490196"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="5" width="18.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.64"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1" s="8">
+    <row r="1" s="8" customFormat="true" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
         <v>9</v>
       </c>
@@ -416,7 +448,7 @@
       <c r="K1" s="7"/>
       <c r="L1" s="7"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="2" s="3">
+    <row r="2" s="3" customFormat="true" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>11</v>
       </c>
@@ -454,7 +486,7 @@
         <v>6</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="3">
+    <row r="3" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="11" t="n">
         <v>1</v>
       </c>
@@ -476,38 +508,28 @@
       <c r="G3" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="H3" s="12" t="inlineStr">
+      <c r="H3" s="12" t="n">
         <f aca="false">G4</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="I3" s="12" t="inlineStr">
+        <v>0.76</v>
+      </c>
+      <c r="I3" s="12" t="n">
         <f aca="false">G5</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="J3" s="12" t="inlineStr">
+        <v>0.35</v>
+      </c>
+      <c r="J3" s="12" t="n">
         <f aca="false">G6</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="K3" s="12" t="inlineStr">
+        <v>0.5</v>
+      </c>
+      <c r="K3" s="12" t="n">
         <f aca="false">G7</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="L3" s="12" t="inlineStr">
+        <v>0.24</v>
+      </c>
+      <c r="L3" s="12" t="n">
         <f aca="false">G8</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="4">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="11" t="n">
         <v>2</v>
       </c>
@@ -532,32 +554,24 @@
       <c r="H4" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="I4" s="12" t="inlineStr">
+      <c r="I4" s="12" t="n">
         <f aca="false">H5</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="J4" s="12" t="inlineStr">
+        <v>0.04</v>
+      </c>
+      <c r="J4" s="12" t="n">
         <f aca="false">H6</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="K4" s="12" t="inlineStr">
+        <v>0.3</v>
+      </c>
+      <c r="K4" s="12" t="n">
         <f aca="false">H7</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="L4" s="12" t="inlineStr">
+        <v>0.36</v>
+      </c>
+      <c r="L4" s="12" t="n">
         <f aca="false">H8</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="5">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="11" t="n">
         <v>3</v>
       </c>
@@ -585,26 +599,20 @@
       <c r="I5" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="J5" s="12" t="inlineStr">
+      <c r="J5" s="12" t="n">
         <f aca="false">I6</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="K5" s="12" t="inlineStr">
+        <v>0.87</v>
+      </c>
+      <c r="K5" s="12" t="n">
         <f aca="false">I7</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="L5" s="12" t="inlineStr">
+        <v>0.62</v>
+      </c>
+      <c r="L5" s="12" t="n">
         <f aca="false">I8</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="6">
+        <v>-0.05</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="11" t="n">
         <v>4</v>
       </c>
@@ -614,7 +622,7 @@
       <c r="C6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="2" t="n">
@@ -635,20 +643,16 @@
       <c r="J6" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="K6" s="12" t="inlineStr">
+      <c r="K6" s="12" t="n">
         <f aca="false">J7</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="L6" s="12" t="inlineStr">
+        <v>0.52</v>
+      </c>
+      <c r="L6" s="12" t="n">
         <f aca="false">J8</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="7">
+        <v>-0.02</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="11" t="n">
         <v>5</v>
       </c>
@@ -658,7 +662,7 @@
       <c r="C7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E7" s="2" t="n">
@@ -682,14 +686,12 @@
       <c r="K7" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="L7" s="12" t="inlineStr">
+      <c r="L7" s="12" t="n">
         <f aca="false">K8</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="8">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="11" t="n">
         <v>6</v>
       </c>
@@ -734,7 +736,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>

<commit_message>
[DROOLS-4900] bump to poi 4 (#714)
</commit_message>
<xml_diff>
--- a/optaplanner-examples/data/investment/import/irrinki_1.xlsx
+++ b/optaplanner-examples/data/investment/import/irrinki_1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="3" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="239" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Parametrization" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,73 +14,78 @@
     <sheet name="AssetClasses" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="21">
   <si>
-    <t>Investment parametrization</t>
-  </si>
-  <si>
-    <t>Standard deviation maximum</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Quantity maximum</t>
-  </si>
-  <si>
-    <t>UK</t>
-  </si>
-  <si>
-    <t>Global</t>
-  </si>
-  <si>
-    <t>Equities</t>
-  </si>
-  <si>
-    <t>Bonds</t>
-  </si>
-  <si>
-    <t>Real Estate</t>
-  </si>
-  <si>
-    <t>Asset class</t>
-  </si>
-  <si>
-    <t>Correlation</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>Region</t>
-  </si>
-  <si>
-    <t>Sector</t>
-  </si>
-  <si>
-    <t>Expected return</t>
-  </si>
-  <si>
-    <t>Standard deviation</t>
-  </si>
-  <si>
-    <t>UK Equities</t>
-  </si>
-  <si>
-    <t>Ex-UK Equities</t>
-  </si>
-  <si>
-    <t>Intermediate Bonds</t>
-  </si>
-  <si>
-    <t>Long-Term Bonds</t>
-  </si>
-  <si>
-    <t>UK Bonds</t>
+    <t xml:space="preserve">Investment parametrization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Standard deviation maximum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quantity maximum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Global</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Equities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bonds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Real Estate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asset class</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Correlation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Region</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expected return</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Standard deviation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UK Equities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ex-UK Equities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intermediate Bonds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Long-Term Bonds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UK Bonds</t>
   </si>
 </sst>
 </file>
@@ -88,42 +93,37 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt formatCode="GENERAL" numFmtId="164"/>
-    <numFmt formatCode="0.00%" numFmtId="165"/>
+    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="0.00%"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <sz val="10"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <sz val="10"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <sz val="10"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <sz val="10"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <charset val="1"/>
-      <family val="2"/>
       <b val="true"/>
       <sz val="10"/>
-    </font>
-    <font>
       <name val="Arial"/>
       <family val="2"/>
-      <sz val="10"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -135,28 +135,28 @@
     </fill>
   </fills>
   <borders count="4">
-    <border diagonalDown="false" diagonalUp="false">
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom style="hair"/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right style="hair"/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right style="hair"/>
       <top/>
@@ -165,63 +165,91 @@
     </border>
   </borders>
   <cellStyleXfs count="20">
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="2" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="4" numFmtId="165" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="3" fillId="0" fontId="4" numFmtId="165" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0"/>
+  <cellXfs count="13">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
-    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
-    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
-    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
-    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -233,21 +261,22 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B2" activeCellId="0" pane="topLeft" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.3058823529412"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.6313725490196"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.64"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1">
+    <row r="1" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="2">
+    <row r="2" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>1</v>
       </c>
@@ -258,7 +287,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="true" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -273,17 +302,18 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C9" activeCellId="0" pane="topLeft" sqref="C9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6313725490196"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.1411764705882"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.6313725490196"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.64"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1" s="3">
+    <row r="1" s="3" customFormat="true" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -291,7 +321,7 @@
         <v>3</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="2">
+    <row r="2" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>4</v>
       </c>
@@ -299,7 +329,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="3">
+    <row r="3" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>5</v>
       </c>
@@ -310,7 +340,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -325,17 +355,18 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B3" activeCellId="0" pane="topLeft" sqref="B3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6313725490196"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.1411764705882"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.6313725490196"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.64"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1" s="3">
+    <row r="1" s="3" customFormat="true" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -343,7 +374,7 @@
         <v>3</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="2">
+    <row r="2" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
@@ -351,7 +382,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="3">
+    <row r="3" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
@@ -359,7 +390,7 @@
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="4">
+    <row r="4" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>8</v>
       </c>
@@ -370,7 +401,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -385,20 +416,21 @@
   </sheetPr>
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B10" activeCellId="0" pane="topLeft" sqref="B10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L29" activeCellId="0" sqref="L29"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.4078431372549"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.4588235294118"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="14.4980392156863"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="14.4980392156863"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="18.0078431372549"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.6313725490196"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="5" width="18.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.64"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1" s="8">
+    <row r="1" s="8" customFormat="true" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
         <v>9</v>
       </c>
@@ -416,7 +448,7 @@
       <c r="K1" s="7"/>
       <c r="L1" s="7"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="2" s="3">
+    <row r="2" s="3" customFormat="true" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>11</v>
       </c>
@@ -454,7 +486,7 @@
         <v>6</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="3">
+    <row r="3" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="11" t="n">
         <v>1</v>
       </c>
@@ -476,38 +508,28 @@
       <c r="G3" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="H3" s="12" t="inlineStr">
+      <c r="H3" s="12" t="n">
         <f aca="false">G4</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="I3" s="12" t="inlineStr">
+        <v>0.76</v>
+      </c>
+      <c r="I3" s="12" t="n">
         <f aca="false">G5</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="J3" s="12" t="inlineStr">
+        <v>0.35</v>
+      </c>
+      <c r="J3" s="12" t="n">
         <f aca="false">G6</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="K3" s="12" t="inlineStr">
+        <v>0.5</v>
+      </c>
+      <c r="K3" s="12" t="n">
         <f aca="false">G7</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="L3" s="12" t="inlineStr">
+        <v>0.24</v>
+      </c>
+      <c r="L3" s="12" t="n">
         <f aca="false">G8</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="4">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="11" t="n">
         <v>2</v>
       </c>
@@ -532,32 +554,24 @@
       <c r="H4" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="I4" s="12" t="inlineStr">
+      <c r="I4" s="12" t="n">
         <f aca="false">H5</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="J4" s="12" t="inlineStr">
+        <v>0.04</v>
+      </c>
+      <c r="J4" s="12" t="n">
         <f aca="false">H6</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="K4" s="12" t="inlineStr">
+        <v>0.3</v>
+      </c>
+      <c r="K4" s="12" t="n">
         <f aca="false">H7</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="L4" s="12" t="inlineStr">
+        <v>0.36</v>
+      </c>
+      <c r="L4" s="12" t="n">
         <f aca="false">H8</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="5">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="11" t="n">
         <v>3</v>
       </c>
@@ -585,26 +599,20 @@
       <c r="I5" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="J5" s="12" t="inlineStr">
+      <c r="J5" s="12" t="n">
         <f aca="false">I6</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="K5" s="12" t="inlineStr">
+        <v>0.87</v>
+      </c>
+      <c r="K5" s="12" t="n">
         <f aca="false">I7</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="L5" s="12" t="inlineStr">
+        <v>0.62</v>
+      </c>
+      <c r="L5" s="12" t="n">
         <f aca="false">I8</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="6">
+        <v>-0.05</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="11" t="n">
         <v>4</v>
       </c>
@@ -614,7 +622,7 @@
       <c r="C6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="2" t="n">
@@ -635,20 +643,16 @@
       <c r="J6" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="K6" s="12" t="inlineStr">
+      <c r="K6" s="12" t="n">
         <f aca="false">J7</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="L6" s="12" t="inlineStr">
+        <v>0.52</v>
+      </c>
+      <c r="L6" s="12" t="n">
         <f aca="false">J8</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="7">
+        <v>-0.02</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="11" t="n">
         <v>5</v>
       </c>
@@ -658,7 +662,7 @@
       <c r="C7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E7" s="2" t="n">
@@ -682,14 +686,12 @@
       <c r="K7" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="L7" s="12" t="inlineStr">
+      <c r="L7" s="12" t="n">
         <f aca="false">K8</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="8">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="11" t="n">
         <v>6</v>
       </c>
@@ -734,7 +736,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>